<commit_message>
offer_agg refactored; ready for data encoding
</commit_message>
<xml_diff>
--- a/data/offer_agg_comparison.xlsx
+++ b/data/offer_agg_comparison.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="6" documentId="8_{36FB71BC-80E8-4C88-BBE4-23520369F242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE3FEC28-42B6-49A5-9E75-6D8E532A8BEE}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="-120" windowWidth="36855" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3:AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,39 +702,39 @@
         <v>132</v>
       </c>
       <c r="K3" t="b">
-        <f>B3=U3</f>
+        <f t="shared" ref="K3:K19" si="0">B3=U3</f>
         <v>1</v>
       </c>
       <c r="L3" t="b">
-        <f>C3=V3</f>
+        <f t="shared" ref="L3:L19" si="1">C3=V3</f>
         <v>1</v>
       </c>
       <c r="M3" t="b">
-        <f>D3=W3</f>
+        <f t="shared" ref="M3:M19" si="2">D3=W3</f>
         <v>1</v>
       </c>
       <c r="N3" t="b">
-        <f>E3=X3</f>
+        <f t="shared" ref="N3:N19" si="3">E3=X3</f>
         <v>1</v>
       </c>
       <c r="O3" t="b">
-        <f>F3=Y3</f>
+        <f t="shared" ref="O3:O19" si="4">F3=Y3</f>
         <v>1</v>
       </c>
       <c r="P3" t="b">
-        <f>G3=Z3</f>
+        <f t="shared" ref="P3:P19" si="5">G3=Z3</f>
         <v>1</v>
       </c>
       <c r="Q3" t="b">
-        <f>H3=AA3</f>
+        <f t="shared" ref="Q3:Q19" si="6">H3=AA3</f>
         <v>1</v>
       </c>
       <c r="R3" t="b">
-        <f>I3=AB3</f>
+        <f t="shared" ref="R3:R19" si="7">I3=AB3</f>
         <v>1</v>
       </c>
       <c r="S3" t="b">
-        <f>J3=AC3</f>
+        <f t="shared" ref="S3:S19" si="8">J3=AC3</f>
         <v>1</v>
       </c>
       <c r="T3" s="6">
@@ -797,39 +797,39 @@
         <v>5</v>
       </c>
       <c r="K4" t="b">
-        <f>B4=U4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L4" t="b">
-        <f>C4=V4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M4" t="b">
-        <f>D4=W4</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N4" t="b">
-        <f>E4=X4</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O4" t="b">
-        <f>F4=Y4</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P4" t="b">
-        <f>G4=Z4</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q4" t="b">
-        <f>H4=AA4</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R4" t="b">
-        <f>I4=AB4</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S4" t="b">
-        <f>J4=AC4</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T4" s="6">
@@ -886,39 +886,39 @@
         <v>2</v>
       </c>
       <c r="K5" t="b">
-        <f>B5=U5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L5" t="b">
-        <f>C5=V5</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M5" t="b">
-        <f>D5=W5</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N5" t="b">
-        <f>E5=X5</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O5" t="b">
-        <f>F5=Y5</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P5" t="b">
-        <f>G5=Z5</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q5" t="b">
-        <f>H5=AA5</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R5" t="b">
-        <f>I5=AB5</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S5" t="b">
-        <f>J5=AC5</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T5" s="6">
@@ -981,39 +981,39 @@
         <v>60</v>
       </c>
       <c r="K6" t="b">
-        <f>B6=U6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L6" t="b">
-        <f>C6=V6</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M6" t="b">
-        <f>D6=W6</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N6" t="b">
-        <f>E6=X6</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O6" t="b">
-        <f>F6=Y6</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P6" t="b">
-        <f>G6=Z6</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q6" t="b">
-        <f>H6=AA6</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R6" t="b">
-        <f>I6=AB6</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S6" t="b">
-        <f>J6=AC6</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T6" s="6">
@@ -1076,39 +1076,39 @@
         <v>3</v>
       </c>
       <c r="K7" t="b">
-        <f>B7=U7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L7" t="b">
-        <f>C7=V7</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M7" t="b">
-        <f>D7=W7</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N7" t="b">
-        <f>E7=X7</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O7" t="b">
-        <f>F7=Y7</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P7" t="b">
-        <f>G7=Z7</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q7" t="b">
-        <f>H7=AA7</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R7" t="b">
-        <f>I7=AB7</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S7" t="b">
-        <f>J7=AC7</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T7" s="6">
@@ -1171,39 +1171,39 @@
         <v>198</v>
       </c>
       <c r="K8" t="b">
-        <f>B8=U8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L8" t="b">
-        <f>C8=V8</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M8" t="b">
-        <f>D8=W8</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N8" t="b">
-        <f>E8=X8</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O8" t="b">
-        <f>F8=Y8</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P8" t="b">
-        <f>G8=Z8</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q8" t="b">
-        <f>H8=AA8</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R8" t="b">
-        <f>I8=AB8</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S8" t="b">
-        <f>J8=AC8</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T8" s="6">
@@ -1272,39 +1272,39 @@
         <v>456</v>
       </c>
       <c r="K9" t="b">
-        <f>B9=U9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L9" t="b">
-        <f>C9=V9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M9" t="b">
-        <f>D9=W9</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N9" t="b">
-        <f>E9=X9</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O9" t="b">
-        <f>F9=Y9</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P9" t="b">
-        <f>G9=Z9</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q9" t="b">
-        <f>H9=AA9</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R9" t="b">
-        <f>I9=AB9</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S9" t="b">
-        <f>J9=AC9</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T9" s="6">
@@ -1373,39 +1373,39 @@
         <v>384</v>
       </c>
       <c r="K10" t="b">
-        <f>B10=U10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L10" t="b">
-        <f>C10=V10</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M10" t="b">
-        <f>D10=W10</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N10" t="b">
-        <f>E10=X10</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O10" t="b">
-        <f>F10=Y10</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P10" t="b">
-        <f>G10=Z10</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q10" t="b">
-        <f>H10=AA10</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R10" t="b">
-        <f>I10=AB10</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S10" t="b">
-        <f>J10=AC10</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T10" s="6">
@@ -1474,39 +1474,39 @@
         <v>510</v>
       </c>
       <c r="K11" t="b">
-        <f>B11=U11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L11" t="b">
-        <f>C11=V11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M11" t="b">
-        <f>D11=W11</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N11" t="b">
-        <f>E11=X11</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O11" t="b">
-        <f>F11=Y11</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P11" t="b">
-        <f>G11=Z11</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q11" t="b">
-        <f>H11=AA11</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R11" t="b">
-        <f>I11=AB11</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S11" t="b">
-        <f>J11=AC11</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T11" s="6">
@@ -1575,39 +1575,39 @@
         <v>522</v>
       </c>
       <c r="K12" t="b">
-        <f>B12=U12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L12" t="b">
-        <f>C12=V12</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M12" t="b">
-        <f>D12=W12</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N12" t="b">
-        <f>E12=X12</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O12" t="b">
-        <f>F12=Y12</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P12" t="b">
-        <f>G12=Z12</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q12" t="b">
-        <f>H12=AA12</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R12" t="b">
-        <f>I12=AB12</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S12" t="b">
-        <f>J12=AC12</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T12" s="6">
@@ -1676,39 +1676,39 @@
         <v>414</v>
       </c>
       <c r="K13" t="b">
-        <f>B13=U13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L13" t="b">
-        <f>C13=V13</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M13" t="b">
-        <f>D13=W13</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N13" t="b">
-        <f>E13=X13</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O13" t="b">
-        <f>F13=Y13</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P13" t="b">
-        <f>G13=Z13</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q13" t="b">
-        <f>H13=AA13</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R13" t="b">
-        <f>I13=AB13</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S13" t="b">
-        <f>J13=AC13</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T13" s="6">
@@ -1777,39 +1777,39 @@
         <v>510</v>
       </c>
       <c r="K14" t="b">
-        <f>B14=U14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L14" t="b">
-        <f>C14=V14</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M14" t="b">
-        <f>D14=W14</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N14" t="b">
-        <f>E14=X14</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O14" t="b">
-        <f>F14=Y14</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P14" t="b">
-        <f>G14=Z14</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q14" t="b">
-        <f>H14=AA14</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R14" t="b">
-        <f>I14=AB14</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S14" t="b">
-        <f>J14=AC14</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T14" s="6">
@@ -1869,39 +1869,39 @@
         <v>5</v>
       </c>
       <c r="K15" t="b">
-        <f>B15=U15</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L15" t="b">
-        <f>C15=V15</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M15" t="b">
-        <f>D15=W15</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N15" t="b">
-        <f>E15=X15</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O15" t="b">
-        <f>F15=Y15</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P15" t="b">
-        <f>G15=Z15</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q15" t="b">
-        <f>H15=AA15</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R15" t="b">
-        <f>I15=AB15</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S15" t="b">
-        <f>J15=AC15</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T15" s="6">
@@ -1964,39 +1964,39 @@
         <v>522</v>
       </c>
       <c r="K16" t="b">
-        <f>B16=U16</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L16" t="b">
-        <f>C16=V16</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M16" t="b">
-        <f>D16=W16</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N16" t="b">
-        <f>E16=X16</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O16" t="b">
-        <f>F16=Y16</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P16" t="b">
-        <f>G16=Z16</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q16" t="b">
-        <f>H16=AA16</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R16" t="b">
-        <f>I16=AB16</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S16" t="b">
-        <f>J16=AC16</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T16" s="6">
@@ -2065,39 +2065,39 @@
         <v>504</v>
       </c>
       <c r="K17" t="b">
-        <f>B17=U17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L17" t="b">
-        <f>C17=V17</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M17" t="b">
-        <f>D17=W17</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N17" t="b">
-        <f>E17=X17</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O17" t="b">
-        <f>F17=Y17</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P17" t="b">
-        <f>G17=Z17</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q17" t="b">
-        <f>H17=AA17</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R17" t="b">
-        <f>I17=AB17</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S17" t="b">
-        <f>J17=AC17</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T17" s="6">
@@ -2157,39 +2157,39 @@
         <v>5</v>
       </c>
       <c r="K18" t="b">
-        <f>B18=U18</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L18" t="b">
-        <f>C18=V18</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M18" t="b">
-        <f>D18=W18</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N18" t="b">
-        <f>E18=X18</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O18" t="b">
-        <f>F18=Y18</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P18" t="b">
-        <f>G18=Z18</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q18" t="b">
-        <f>H18=AA18</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R18" t="b">
-        <f>I18=AB18</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S18" t="b">
-        <f>J18=AC18</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T18" s="6">
@@ -2252,39 +2252,39 @@
         <v>576</v>
       </c>
       <c r="K19" t="b">
-        <f>B19=U19</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L19" t="b">
-        <f>C19=V19</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M19" t="b">
-        <f>D19=W19</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N19" t="b">
-        <f>E19=X19</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O19" t="b">
-        <f>F19=Y19</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P19" t="b">
-        <f>G19=Z19</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q19" t="b">
-        <f>H19=AA19</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R19" t="b">
-        <f>I19=AB19</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S19" t="b">
-        <f>J19=AC19</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T19" s="6">

</xml_diff>